<commit_message>
Bug fix for LipidHome.json. Add more screenshot to user guide page
</commit_message>
<xml_diff>
--- a/doc/sample_data/input/LipidLynxX_test.xlsx
+++ b/doc/sample_data/input/LipidLynxX_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SysMedOs\LipidLynxX\doc\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SysMedOs\LipidLynxX\doc\sample_data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{720E11A8-1685-4748-B2E9-D675E512EB28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEF5886-C835-47B6-8FC0-4570564CFCFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LipidLynxX_test" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1297,12 +1297,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1950,5 +1963,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>